<commit_message>
5.1 (based on branch 3.x)
</commit_message>
<xml_diff>
--- a/board/bom.xlsx
+++ b/board/bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="99">
   <si>
     <t>Comment</t>
   </si>
@@ -78,13 +78,46 @@
     <t>C2</t>
   </si>
   <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>CAP_0402</t>
+  </si>
+  <si>
+    <t>C1546</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
     <t>470pF</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>CAP_0402</t>
+    <t>C12</t>
   </si>
   <si>
     <t>C1537</t>
@@ -93,45 +126,12 @@
     <t>22pF</t>
   </si>
   <si>
-    <t>C4</t>
+    <t>C13</t>
   </si>
   <si>
     <t>C1555</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C1546</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
     <t>C14</t>
   </si>
   <si>
@@ -168,6 +168,15 @@
     <t>C25</t>
   </si>
   <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
@@ -201,7 +210,7 @@
     <t>R3</t>
   </si>
   <si>
-    <t>200R</t>
+    <t>100R</t>
   </si>
   <si>
     <t>R4</t>
@@ -210,7 +219,7 @@
     <t>0402_x4</t>
   </si>
   <si>
-    <t>C2011</t>
+    <t>C48442</t>
   </si>
   <si>
     <t>R5</t>
@@ -261,49 +270,110 @@
     <t>C5358</t>
   </si>
   <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>TSOP-32/8x14+20x0.5</t>
+  </si>
+  <si>
+    <t>C261875</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SOP-48/8.1x0.5</t>
+  </si>
+  <si>
+    <t>C5531</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>TSSOP-24</t>
+  </si>
+  <si>
+    <t>C7859</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>C347229</t>
+  </si>
+  <si>
+    <t>EPM1270T144C5N</t>
+  </si>
+  <si>
+    <t>LD1117-3.3</t>
+  </si>
+  <si>
+    <t>LY62L2568LL-55LLI</t>
+  </si>
+  <si>
+    <t>74ALVC164245DGG:11</t>
+  </si>
+  <si>
+    <t>SN74LVC4245APWR</t>
+  </si>
+  <si>
+    <t>DIODE</t>
+  </si>
+  <si>
+    <t>FM18L08</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
     <t>U3</t>
   </si>
   <si>
-    <t>TSOP-32/8x14+20x0.5</t>
-  </si>
-  <si>
-    <t>C261875</t>
-  </si>
-  <si>
-    <t>3.3V</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOT223-4</t>
-  </si>
-  <si>
-    <t>C6186</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOP-48/8.1x0.5</t>
-  </si>
-  <si>
-    <t>C5531</t>
-  </si>
-  <si>
-    <t>U6</t>
+    <t>S29GL01GP</t>
+  </si>
+  <si>
+    <t>TSOP-56</t>
+  </si>
+  <si>
+    <t>SOIC-28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -369,17 +439,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -652,15 +724,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" activeCellId="2" sqref="A28:XFD28 A29:XFD29 A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
@@ -724,147 +796,147 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>27</v>
@@ -873,12 +945,12 @@
         <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>28</v>
@@ -887,12 +959,12 @@
         <v>11</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>29</v>
@@ -901,12 +973,12 @@
         <v>11</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>30</v>
@@ -915,12 +987,12 @@
         <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>31</v>
@@ -929,12 +1001,12 @@
         <v>11</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>32</v>
@@ -943,12 +1015,12 @@
         <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>33</v>
@@ -957,12 +1029,12 @@
         <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>34</v>
@@ -971,12 +1043,12 @@
         <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>35</v>
@@ -985,12 +1057,12 @@
         <v>11</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>36</v>
@@ -999,12 +1071,12 @@
         <v>11</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>37</v>
@@ -1013,12 +1085,12 @@
         <v>11</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>38</v>
@@ -1027,322 +1099,427 @@
         <v>11</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="3"/>
+      <c r="A27" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="C30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="C46" s="3" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C49" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3" t="s">
+    <row r="53" spans="1:4">
+      <c r="A53" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3" t="s">
+    <row r="54" spans="1:4">
+      <c r="A54" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>